<commit_message>
cm: update oncho pre stop form
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Cameroon/cm_oncho_pre_stop_1_202309_village.xlsx
+++ b/ONCHO/Impact Assessments/Cameroon/cm_oncho_pre_stop_1_202309_village.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Cameroon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486B936A-130D-46F9-84F4-6447BE599E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61FE7CF-C4C7-4562-9597-2A802382F749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4360" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="490">
   <si>
     <t>type</t>
   </si>
@@ -1604,17 +1604,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1950,8 +1940,8 @@
   </sheetPr>
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,9 +2160,7 @@
       <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -2221,7 +2209,7 @@
   </sheetPr>
   <dimension ref="A1:F776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D1" activeCellId="1" sqref="B1:B1048576 D1:F1048576"/>
     </sheetView>

</xml_diff>